<commit_message>
Fix: Add matrizes de similaridade
</commit_message>
<xml_diff>
--- a/RBC/Modelo_RBC.xlsx
+++ b/RBC/Modelo_RBC.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acanixz\workspace\UNIVALI\IA_Univali\RBC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288CF569-CFF8-457A-8A32-A127BD4C4B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F74771C-D255-41CD-8656-6664B8C9AE64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2070" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="435" windowWidth="16410" windowHeight="10830" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Atributos" sheetId="1" r:id="rId1"/>
     <sheet name="Pesos e Metricas" sheetId="2" r:id="rId2"/>
+    <sheet name="Matrizes Correlação" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Pesos e Metricas'!$A$1:$D$13</definedName>
@@ -42,7 +43,7 @@
     <author>Acanixz</author>
   </authors>
   <commentList>
-    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{0675C8A9-30EF-4189-8E9B-ED4ED759F98E}">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{6D4AD44B-A2D9-4D02-A374-8E402F61C067}">
       <text>
         <r>
           <rPr>
@@ -50,7 +51,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Acanixz:</t>
         </r>
@@ -59,13 +60,263 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 |x1 - x2| / (max - min) = grau de diferença a partir de dois valores, divido pelo valor (maximo-minimo) do atributo
 O valor é então subtraido de 1 para obter o grau de similaridade
 1 = Idêntico
 0 = Completamente diferente</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Acanixz</author>
+  </authors>
+  <commentList>
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{E1258F32-F870-49C3-B6F4-BC8FC243EB37}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Acanixz:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Tipo de dor no peito</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{F37768D7-BDAF-4905-8C7E-95352E79D33D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Acanixz:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Assintomático</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P5" authorId="0" shapeId="0" xr:uid="{7132D38F-F95B-4F60-8890-69B83AAACA64}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Acanixz:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ascendente</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{1BC6B204-05CA-4778-AF45-456C2FF8FAEA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Acanixz:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Angina Atípica</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J6" authorId="0" shapeId="0" xr:uid="{5A755F56-CA0A-4186-A999-78AFC2DEDB36}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Acanixz:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Anormalidade da onda ST-T</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P6" authorId="0" shapeId="0" xr:uid="{41D952DF-9EE1-47C5-89E9-E88147DEF24B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Acanixz:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Plana</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{ECC620F4-D6D4-4BE1-AC9F-E41E4D646E8D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Acanixz:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Dor Não Anginosa</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J7" authorId="0" shapeId="0" xr:uid="{E6F38B01-5E9E-4996-AEBA-23A2E71E4D54}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Acanixz:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Hipertrofia ventricular esquerda provável ou definitiva</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P7" authorId="0" shapeId="0" xr:uid="{4FDA873E-7232-481C-9521-C5AB5732A5B2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Acanixz:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Descendente</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{F36A496A-0BB8-4E67-BF1E-4BE2DEE5675D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Acanixz:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Angina Típica</t>
         </r>
       </text>
     </comment>
@@ -74,7 +325,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="57">
   <si>
     <t>Age</t>
   </si>
@@ -212,13 +463,46 @@
   </si>
   <si>
     <t>Categorico</t>
+  </si>
+  <si>
+    <t>ASY</t>
+  </si>
+  <si>
+    <t>ATA</t>
+  </si>
+  <si>
+    <t>NAP</t>
+  </si>
+  <si>
+    <t>TA</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>LVH</t>
+  </si>
+  <si>
+    <t>Up</t>
+  </si>
+  <si>
+    <t>Flat</t>
+  </si>
+  <si>
+    <t>Down</t>
+  </si>
+  <si>
+    <t>matriz de similaridade manual</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,28 +525,49 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Segoe UI"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Segoe UI"/>
-      <charset val="1"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -285,17 +590,175 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -604,7 +1067,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,16 +1247,16 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -807,14 +1270,14 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -854,9 +1317,9 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -938,9 +1401,9 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>22</v>
       </c>
     </row>
@@ -980,9 +1443,9 @@
         <v>0.03</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1010,4 +1473,222 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84E66FA7-6B62-4D0E-9BD1-ECD76C2B634D}">
+  <dimension ref="C2:S8"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="3:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="15"/>
+      <c r="J3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="15"/>
+      <c r="P3" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="15"/>
+    </row>
+    <row r="4" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C4" s="5"/>
+      <c r="D4" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="R4" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="S4" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="F5">
+        <v>0.33333333333333343</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>0.5</v>
+      </c>
+      <c r="M5" s="7">
+        <v>0</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>0.5</v>
+      </c>
+      <c r="S5" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C6" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6">
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0.33333333333333343</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6">
+        <v>0.5</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q6">
+        <v>0.5</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6" s="7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7">
+        <v>0.33333333333333343</v>
+      </c>
+      <c r="E7">
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="K7" s="9">
+        <v>0</v>
+      </c>
+      <c r="L7" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="M7" s="10">
+        <v>1</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q7" s="9">
+        <v>0</v>
+      </c>
+      <c r="R7" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="S7" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0.33333333333333343</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="G8" s="10">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="P3:S3"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>